<commit_message>
feat: experimenting with randomization
</commit_message>
<xml_diff>
--- a/data/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
+++ b/data/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70867FB-18E5-824E-9554-3732ED11527E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BF91DF-EC3B-1842-BDE1-E34A7D6DF4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31000" yWindow="860" windowWidth="29920" windowHeight="18660" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
+    <workbookView xWindow="-29920" yWindow="5340" windowWidth="29920" windowHeight="18660" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>text_type</t>
   </si>
   <si>
-    <t>text_annotated_spans</t>
-  </si>
-  <si>
     <t>question_id</t>
   </si>
   <si>
@@ -104,19 +101,7 @@
     <t>target</t>
   </si>
   <si>
-    <t>distractor_1</t>
-  </si>
-  <si>
-    <t>distractor_2</t>
-  </si>
-  <si>
-    <t>distractor_3</t>
-  </si>
-  <si>
     <t>target_span_text</t>
-  </si>
-  <si>
-    <t>distractor_1_span_text</t>
   </si>
   <si>
     <t>George Eliot - Middlemarch</t>
@@ -297,6 +282,21 @@
   </si>
   <si>
     <t>toy_text_practice_1toy_text_4</t>
+  </si>
+  <si>
+    <t>distractor_a</t>
+  </si>
+  <si>
+    <t>text_with_annotated_spans</t>
+  </si>
+  <si>
+    <t>distractor_span_text</t>
+  </si>
+  <si>
+    <t>distractor_b</t>
+  </si>
+  <si>
+    <t>distractor_c</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899C6EA3-68FC-004D-97A8-DCDE2573704E}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -795,31 +795,31 @@
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="M1" s="7" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="356" x14ac:dyDescent="0.2">
@@ -830,37 +830,37 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="272" x14ac:dyDescent="0.2">
@@ -871,31 +871,31 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>37</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="272" x14ac:dyDescent="0.2">
@@ -906,37 +906,37 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="L4" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="221" x14ac:dyDescent="0.2">
@@ -947,37 +947,37 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="221" x14ac:dyDescent="0.2">
@@ -988,37 +988,37 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: shuffle answer options for each session
</commit_message>
<xml_diff>
--- a/data/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
+++ b/data/stimuli_toy/multipleye_comprehension_questions_toy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BF91DF-EC3B-1842-BDE1-E34A7D6DF4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803F43B-8644-874A-8B5B-F8F4918AA6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29920" yWindow="5340" windowWidth="29920" windowHeight="18660" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{BF0A98E9-F8D9-4949-AD77-1583D2976307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={CACC8550-F5E4-2046-8B96-A9DB1E27561A}</author>
-    <author>tc={616F3D29-E64B-F54B-B753-D6FC9C73ACDA}</author>
     <author>tc={0026CF7B-0CC9-734D-B302-AF1097768FE9}</author>
   </authors>
   <commentList>
@@ -51,15 +50,7 @@
     The first few columns make it easier for me to process while creating the images but should not be touched :) </t>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{616F3D29-E64B-F54B-B753-D6FC9C73ACDA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I think it would be easiest if you could add a $..$ around the target span and $$..$$ around the distractor_1 span, etc. (if applicable) —&gt; then I can very easily compute the word indices and add it to the air files. Counting the indices by hand it too tedious.. but if you also add the actual text (see other columns) I can double check that all is correct.</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="2" shapeId="0" xr:uid="{0026CF7B-0CC9-734D-B302-AF1097768FE9}">
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{0026CF7B-0CC9-734D-B302-AF1097768FE9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -86,12 +77,6 @@
     <t>experiment</t>
   </si>
   <si>
-    <t>text_type</t>
-  </si>
-  <si>
-    <t>question_id</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
@@ -99,9 +84,6 @@
   </si>
   <si>
     <t>target</t>
-  </si>
-  <si>
-    <t>target_span_text</t>
   </si>
   <si>
     <t>George Eliot - Middlemarch</t>
@@ -281,29 +263,41 @@
     <t>toy_text_3</t>
   </si>
   <si>
-    <t>toy_text_practice_1toy_text_4</t>
-  </si>
-  <si>
     <t>distractor_a</t>
   </si>
   <si>
-    <t>text_with_annotated_spans</t>
-  </si>
-  <si>
-    <t>distractor_span_text</t>
-  </si>
-  <si>
     <t>distractor_b</t>
   </si>
   <si>
     <t>distractor_c</t>
+  </si>
+  <si>
+    <t>stimulus_text_with_annotated_spans</t>
+  </si>
+  <si>
+    <t>stimulus_type</t>
+  </si>
+  <si>
+    <t>target_span_target_distractor_a_text</t>
+  </si>
+  <si>
+    <t>snippet_no</t>
+  </si>
+  <si>
+    <t>condition_no</t>
+  </si>
+  <si>
+    <t>question_no</t>
+  </si>
+  <si>
+    <t>distractor_span_distractor_b_text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +346,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -427,6 +428,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,9 +457,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -491,7 +497,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -597,7 +603,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -739,7 +745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,10 +756,7 @@
   <threadedComment ref="A1" dT="2023-10-06T13:49:43.10" personId="{748F7033-6D7B-E748-9F66-10D69C5A4C41}" id="{CACC8550-F5E4-2046-8B96-A9DB1E27561A}">
     <text xml:space="preserve">The first few columns make it easier for me to process while creating the images but should not be touched :) </text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2023-10-06T13:53:29.21" personId="{748F7033-6D7B-E748-9F66-10D69C5A4C41}" id="{616F3D29-E64B-F54B-B753-D6FC9C73ACDA}">
-    <text>I think it would be easiest if you could add a $..$ around the target span and $$..$$ around the distractor_1 span, etc. (if applicable) —&gt; then I can very easily compute the word indices and add it to the air files. Counting the indices by hand it too tedious.. but if you also add the actual text (see other columns) I can double check that all is correct.</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2023-10-06T13:47:01.97" personId="{748F7033-6D7B-E748-9F66-10D69C5A4C41}" id="{0026CF7B-0CC9-734D-B302-AF1097768FE9}">
+  <threadedComment ref="I1" dT="2023-10-06T13:47:01.97" personId="{748F7033-6D7B-E748-9F66-10D69C5A4C41}" id="{0026CF7B-0CC9-734D-B302-AF1097768FE9}">
     <text>Here it would be important to have a finite set of options (ideally something that is easy to machine-read, like local_literal_1, global_2, etc.)</text>
   </threadedComment>
 </ThreadedComments>
@@ -761,281 +764,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899C6EA3-68FC-004D-97A8-DCDE2573704E}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="40.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" customWidth="1"/>
-    <col min="13" max="13" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1"/>
+    <col min="15" max="15" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="J1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>43</v>
+      <c r="O1" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="356" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="356" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="M4" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="221" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="221" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>14</v>
+      <c r="O5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="221" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>14</v>
-      </c>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="E6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>